<commit_message>
disable button as needed
</commit_message>
<xml_diff>
--- a/TestScenarios/env2_scenario2.xlsx
+++ b/TestScenarios/env2_scenario2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richard\PycharmProjects\PredictedHeatStrainModel\TestScenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729D4A13-616D-4415-8766-358BF044510D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E280E7-9160-4314-815B-B054A4CBC206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EF479299-A3B3-42BD-BFF1-2CDB4DD4E671}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{EF479299-A3B3-42BD-BFF1-2CDB4DD4E671}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="2" r:id="rId1"/>
@@ -702,7 +702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D67D1F53-EF0F-4BDB-8291-1D55709DE8B4}">
   <dimension ref="A1:S141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -711,7 +711,7 @@
     <col min="6" max="6" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="39" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="26.25" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -2746,8 +2746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9989D48-04BF-4F65-BE7B-33F1E68272E0}">
   <dimension ref="A1:L123"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:L52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>